<commit_message>
Handler now using correct html files + some style changes; updated DummyData
</commit_message>
<xml_diff>
--- a/DummyData/DummyData.xlsx
+++ b/DummyData/DummyData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Repository\SocialServ\DummyData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1298532-C2FF-4B84-B875-3C9DBD9D40BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B68E7D-F556-45DB-96D2-B2F17A4A1772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{521E5B70-F916-4F4E-9455-AE6D958978B2}"/>
   </bookViews>
@@ -427,7 +427,7 @@
     <t>hashed_password</t>
   </si>
   <si>
-    <t>$2b$12$fJZoLTiqMWOwWVwjot1a3eFplVcHrD2KkSXEWlpLYqbzUE982j74W</t>
+    <t>$2a$12$wAjivtgOA8ghj4wU6.P1weHsvGfLWfWaeaW3RKrST5gt72smmd5hW</t>
   </si>
 </sst>
 </file>
@@ -794,7 +794,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D2" sqref="D2:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated post and repost templates + closes #23 fixed testdata bug
</commit_message>
<xml_diff>
--- a/DummyData/DummyData.xlsx
+++ b/DummyData/DummyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Repository\SocialServ\DummyData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B68E7D-F556-45DB-96D2-B2F17A4A1772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499D66DE-DD3D-4CCE-8C00-313576294D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{521E5B70-F916-4F4E-9455-AE6D958978B2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{521E5B70-F916-4F4E-9455-AE6D958978B2}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="129">
   <si>
     <t>username</t>
   </si>
@@ -338,9 +338,6 @@
   </si>
   <si>
     <t>admin, zunairah.philip, guto.gould, kasim.roberts, arun.tanner, madiha.proctor, soraya.oneal, hattie.blair, jacques.seymour, shabaz.russell, cherise.mcdowell</t>
-  </si>
-  <si>
-    <t>null</t>
   </si>
   <si>
     <t>admin, hattie.blair, soraya.oneal, shabaz.russell</t>
@@ -793,7 +790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EA9BD4A-273A-471B-8064-DC483569FE45}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D12"/>
     </sheetView>
   </sheetViews>
@@ -815,7 +812,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -829,7 +826,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -843,7 +840,7 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -857,7 +854,7 @@
         <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -871,7 +868,7 @@
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -885,7 +882,7 @@
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -899,7 +896,7 @@
         <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -913,7 +910,7 @@
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -927,7 +924,7 @@
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -941,7 +938,7 @@
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -955,7 +952,7 @@
         <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -969,7 +966,7 @@
         <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1108,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E4DB95-02F4-42BE-94DF-ACFEBEF32587}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1151,10 +1148,7 @@
         <v>43731</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1165,7 +1159,7 @@
         <v>43925</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D3" t="s">
         <v>77</v>
@@ -1179,10 +1173,7 @@
         <v>44020</v>
       </c>
       <c r="C4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D4" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1193,10 +1184,7 @@
         <v>43928</v>
       </c>
       <c r="C5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D5" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1207,7 +1195,7 @@
         <v>44104</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" t="s">
         <v>77</v>
@@ -1221,7 +1209,7 @@
         <v>44231</v>
       </c>
       <c r="C7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D7" t="s">
         <v>76</v>
@@ -1235,13 +1223,13 @@
         <v>44083</v>
       </c>
       <c r="C8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D8" t="s">
         <v>75</v>
       </c>
       <c r="H8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1252,10 +1240,7 @@
         <v>43831</v>
       </c>
       <c r="C9" t="s">
-        <v>112</v>
-      </c>
-      <c r="D9" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1266,7 +1251,7 @@
         <v>43863</v>
       </c>
       <c r="C10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D10" t="s">
         <v>77</v>
@@ -1280,7 +1265,7 @@
         <v>44229</v>
       </c>
       <c r="C11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D11" t="s">
         <v>76</v>
@@ -1294,10 +1279,7 @@
         <v>43919</v>
       </c>
       <c r="C12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D12" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1308,7 +1290,7 @@
         <v>44015</v>
       </c>
       <c r="C13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D13" t="s">
         <v>77</v>
@@ -1322,7 +1304,7 @@
         <v>44381</v>
       </c>
       <c r="C14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D14" t="s">
         <v>76</v>
@@ -1336,10 +1318,7 @@
         <v>44464</v>
       </c>
       <c r="C15" t="s">
-        <v>119</v>
-      </c>
-      <c r="D15" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1350,7 +1329,7 @@
         <v>44309</v>
       </c>
       <c r="C16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D16" t="s">
         <v>78</v>
@@ -1364,7 +1343,7 @@
         <v>44308</v>
       </c>
       <c r="C17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D17" t="s">
         <v>78</v>
@@ -1378,7 +1357,7 @@
         <v>44435</v>
       </c>
       <c r="C18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D18" t="s">
         <v>78</v>
@@ -1392,10 +1371,7 @@
         <v>44316</v>
       </c>
       <c r="C19" t="s">
-        <v>120</v>
-      </c>
-      <c r="D19" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1406,7 +1382,7 @@
         <v>43862</v>
       </c>
       <c r="C20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D20" t="s">
         <v>77</v>
@@ -1420,7 +1396,7 @@
         <v>44228</v>
       </c>
       <c r="C21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D21" t="s">
         <v>76</v>
@@ -1434,7 +1410,7 @@
         <v>44307</v>
       </c>
       <c r="C22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D22" t="s">
         <v>78</v>
@@ -1448,7 +1424,7 @@
         <v>44258</v>
       </c>
       <c r="C23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D23" t="s">
         <v>76</v>
@@ -1462,10 +1438,7 @@
         <v>44442</v>
       </c>
       <c r="C24" t="s">
-        <v>122</v>
-      </c>
-      <c r="D24" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1476,10 +1449,7 @@
         <v>44443</v>
       </c>
       <c r="C25" t="s">
-        <v>123</v>
-      </c>
-      <c r="D25" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1490,7 +1460,7 @@
         <v>44259</v>
       </c>
       <c r="C26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D26" t="s">
         <v>76</v>
@@ -1504,10 +1474,7 @@
         <v>44377</v>
       </c>
       <c r="C27" t="s">
-        <v>124</v>
-      </c>
-      <c r="D27" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1932,7 +1899,7 @@
         <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>